<commit_message>
Adding alternate excel reader
</commit_message>
<xml_diff>
--- a/Interview/src/main/java/com/amit/web/testData/TestData.xlsx
+++ b/Interview/src/main/java/com/amit/web/testData/TestData.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Selenium\Interview\src\main\java\com\amit\web\testData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\Interview\src\main\java\com\amit\web\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{D3748419-1A7F-4AAD-AD21-5905EAE57972}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9048" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>

</xml_diff>

<commit_message>
Revised learning selenium and java
</commit_message>
<xml_diff>
--- a/Interview/src/main/java/com/amit/web/testData/TestData.xlsx
+++ b/Interview/src/main/java/com/amit/web/testData/TestData.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\Interview\src\main\java\com\amit\web\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{D3748419-1A7F-4AAD-AD21-5905EAE57972}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{57DB87A8-C3E0-46BA-B02D-6F761D547C94}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9048" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9048" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="LoginTestData" sheetId="1" r:id="rId1"/>
-    <sheet name="BullCartelData" sheetId="2" r:id="rId2"/>
-    <sheet name="DBTesting" sheetId="3" r:id="rId3"/>
+    <sheet name="SingleLogin" sheetId="4" r:id="rId1"/>
+    <sheet name="LoginTestData" sheetId="1" r:id="rId2"/>
+    <sheet name="BullCartelData" sheetId="2" r:id="rId3"/>
+    <sheet name="DBTesting" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="11">
   <si>
     <t>userName</t>
   </si>
@@ -411,6 +412,51 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C80944B-0F01-46BA-BCA3-1351D9D68297}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="24.796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.19921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.69921875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{F21E06F4-B1EE-4603-A85F-37B23B6BF8F5}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C6"/>
   <sheetViews>
@@ -502,7 +548,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43893380-BF53-4CCD-861E-0AF81A5D7C7C}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -554,11 +600,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1323F46-A380-4401-9713-2595E5FAA89F}">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
New automation practice files and GS interview prep files
</commit_message>
<xml_diff>
--- a/Interview/src/main/java/com/amit/web/testData/TestData.xlsx
+++ b/Interview/src/main/java/com/amit/web/testData/TestData.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\Interview\src\main\java\com\amit\web\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6D276FF-3618-4337-9350-53C51B4FCC29}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3D45441-E8C3-47BB-AA78-4171DB5436C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SingleLogin" sheetId="4" r:id="rId1"/>
     <sheet name="LoginTestData" sheetId="1" r:id="rId2"/>
     <sheet name="DBTesting" sheetId="3" r:id="rId3"/>
+    <sheet name="HomePage" sheetId="5" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150000"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="18">
   <si>
     <t>userName</t>
   </si>
@@ -69,6 +70,25 @@
   </si>
   <si>
     <t>n</t>
+  </si>
+  <si>
+    <t>SearchText</t>
+  </si>
+  <si>
+    <t>SUMMER DRESSES</t>
+  </si>
+  <si>
+    <t>SearchTextResult</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Printed Summer Dress
+</t>
+  </si>
+  <si>
+    <t>SearchText1</t>
+  </si>
+  <si>
+    <t>Chiffon</t>
   </si>
 </sst>
 </file>
@@ -127,13 +147,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -417,9 +441,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C80944B-0F01-46BA-BCA3-1351D9D68297}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
@@ -581,4 +603,46 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72F4EC60-0D98-4F0A-A78B-4CCDDC5CDB97}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.19921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.8984375" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>